<commit_message>
task data added in the new task file
</commit_message>
<xml_diff>
--- a/da20_excel_task1.xlsx
+++ b/da20_excel_task1.xlsx
@@ -1,26 +1,120 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28827"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DA20\Git_hub\da20_excel_task1\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01BEACA7-226F-4906-882A-FF0B48592D8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+  <si>
+    <t>tax</t>
+  </si>
+  <si>
+    <t>tv</t>
+  </si>
+  <si>
+    <t>mobile</t>
+  </si>
+  <si>
+    <t>speaker</t>
+  </si>
+  <si>
+    <t>headphone</t>
+  </si>
+  <si>
+    <t>laptop</t>
+  </si>
+  <si>
+    <t>total</t>
+  </si>
+  <si>
+    <t>total_after_tax</t>
+  </si>
+  <si>
+    <t>Rank.avg</t>
+  </si>
+  <si>
+    <t>Rank.eq</t>
+  </si>
+  <si>
+    <t>Rank</t>
+  </si>
+  <si>
+    <t>lg</t>
+  </si>
+  <si>
+    <t>smsung</t>
+  </si>
+  <si>
+    <t>apple</t>
+  </si>
+  <si>
+    <t>sony</t>
+  </si>
+  <si>
+    <t>task</t>
+  </si>
+  <si>
+    <t>haier1</t>
+  </si>
+  <si>
+    <t>haier2</t>
+  </si>
+  <si>
+    <t>mi</t>
+  </si>
+  <si>
+    <t>Calculation</t>
+  </si>
+  <si>
+    <t>Average</t>
+  </si>
+  <si>
+    <t>min</t>
+  </si>
+  <si>
+    <t>max</t>
+  </si>
+  <si>
+    <t>da20_excel_task1</t>
+  </si>
+</sst>
+</file>
+
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -28,16 +122,53 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.749992370372631"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.499984740745262"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -45,12 +176,81 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -330,13 +530,430 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="C4:P19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N17" sqref="N17"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="5" width="9.140625" style="1"/>
+    <col min="6" max="6" width="11.7109375" style="1" customWidth="1"/>
+    <col min="7" max="8" width="9.140625" style="1"/>
+    <col min="9" max="9" width="11.140625" style="1" customWidth="1"/>
+    <col min="10" max="11" width="9.140625" style="1"/>
+    <col min="12" max="12" width="13.28515625" style="1" customWidth="1"/>
+    <col min="13" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="J4" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="K4" s="3">
+        <v>0.05</v>
+      </c>
+    </row>
+    <row r="5" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="C5" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="F7" s="4" t="s">
+        <v>1</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="I7" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="J7" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="K7" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="L7" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="M7" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="N7" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="O7" s="4" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="F8" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G8" s="6">
+        <v>40</v>
+      </c>
+      <c r="H8" s="6">
+        <v>67</v>
+      </c>
+      <c r="I8" s="6">
+        <v>78</v>
+      </c>
+      <c r="J8" s="6">
+        <v>0</v>
+      </c>
+      <c r="K8" s="7">
+        <f>SUM(G8:J8)</f>
+        <v>185</v>
+      </c>
+      <c r="L8" s="6">
+        <f>K8+(K8*$K$4)</f>
+        <v>194.25</v>
+      </c>
+      <c r="M8" s="6">
+        <f>_xlfn.RANK.AVG(L8,L$8:L$14,1)</f>
+        <v>1</v>
+      </c>
+      <c r="N8" s="6">
+        <f>_xlfn.RANK.EQ(L8,L$8:L$14,1)</f>
+        <v>1</v>
+      </c>
+      <c r="O8" s="6">
+        <f>RANK(M8,M$8:M$14,1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="F9" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G9" s="6">
+        <v>77</v>
+      </c>
+      <c r="H9" s="6">
+        <v>88</v>
+      </c>
+      <c r="I9" s="6">
+        <v>55</v>
+      </c>
+      <c r="J9" s="6">
+        <v>66</v>
+      </c>
+      <c r="K9" s="7">
+        <f>SUM(G9:J9)</f>
+        <v>286</v>
+      </c>
+      <c r="L9" s="6">
+        <f t="shared" ref="L9:L17" si="0">K9+(K9*$K$4)</f>
+        <v>300.3</v>
+      </c>
+      <c r="M9" s="6">
+        <f t="shared" ref="M9:M14" si="1">_xlfn.RANK.AVG(L9,L$8:L$14,1)</f>
+        <v>6</v>
+      </c>
+      <c r="N9" s="6">
+        <f t="shared" ref="N9:N14" si="2">_xlfn.RANK.EQ(L9,L$8:L$14,1)</f>
+        <v>6</v>
+      </c>
+      <c r="O9" s="6">
+        <f t="shared" ref="O9:O14" si="3">RANK(M9,M$8:M$14,1)</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="F10" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G10" s="6">
+        <v>66</v>
+      </c>
+      <c r="H10" s="6">
+        <v>88</v>
+      </c>
+      <c r="I10" s="6">
+        <v>44</v>
+      </c>
+      <c r="J10" s="6">
+        <v>159</v>
+      </c>
+      <c r="K10" s="7">
+        <f t="shared" ref="K10:K14" si="4">SUM(G10:J10)</f>
+        <v>357</v>
+      </c>
+      <c r="L10" s="6">
+        <f t="shared" si="0"/>
+        <v>374.85</v>
+      </c>
+      <c r="M10" s="6">
+        <f>_xlfn.RANK.AVG(L10,L$8:L$14,1)</f>
+        <v>7</v>
+      </c>
+      <c r="N10" s="6">
+        <f>_xlfn.RANK.EQ(L10,L$8:L$14,1)</f>
+        <v>7</v>
+      </c>
+      <c r="O10" s="6">
+        <f t="shared" si="3"/>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="F11" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="G11" s="6">
+        <v>54</v>
+      </c>
+      <c r="H11" s="6">
+        <v>76</v>
+      </c>
+      <c r="I11" s="6">
+        <v>65</v>
+      </c>
+      <c r="J11" s="6">
+        <v>0</v>
+      </c>
+      <c r="K11" s="7">
+        <f t="shared" si="4"/>
+        <v>195</v>
+      </c>
+      <c r="L11" s="6">
+        <f t="shared" si="0"/>
+        <v>204.75</v>
+      </c>
+      <c r="M11" s="6">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
+      <c r="N11" s="6">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="O11" s="6">
+        <f t="shared" si="3"/>
+        <v>2</v>
+      </c>
+      <c r="P11" s="1" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="12" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="F12" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="G12" s="6">
+        <v>76</v>
+      </c>
+      <c r="H12" s="6">
+        <v>98</v>
+      </c>
+      <c r="I12" s="6">
+        <v>88</v>
+      </c>
+      <c r="J12" s="6">
+        <v>0</v>
+      </c>
+      <c r="K12" s="7">
+        <f>SUM(G12:J12)</f>
+        <v>262</v>
+      </c>
+      <c r="L12" s="6">
+        <f t="shared" si="0"/>
+        <v>275.10000000000002</v>
+      </c>
+      <c r="M12" s="6">
+        <f t="shared" si="1"/>
+        <v>4.5</v>
+      </c>
+      <c r="N12" s="6">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="O12" s="6">
+        <f t="shared" si="3"/>
+        <v>4</v>
+      </c>
+      <c r="P12" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="F13" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="G13" s="6">
+        <v>76</v>
+      </c>
+      <c r="H13" s="6">
+        <v>88</v>
+      </c>
+      <c r="I13" s="6">
+        <v>98</v>
+      </c>
+      <c r="J13" s="6">
+        <v>0</v>
+      </c>
+      <c r="K13" s="7">
+        <f t="shared" si="4"/>
+        <v>262</v>
+      </c>
+      <c r="L13" s="6">
+        <f t="shared" si="0"/>
+        <v>275.10000000000002</v>
+      </c>
+      <c r="M13" s="6">
+        <f t="shared" si="1"/>
+        <v>4.5</v>
+      </c>
+      <c r="N13" s="6">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="O13" s="6">
+        <f t="shared" si="3"/>
+        <v>4</v>
+      </c>
+      <c r="P13" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="14" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="F14" s="5" t="s">
+        <v>18</v>
+      </c>
+      <c r="G14" s="6">
+        <v>76</v>
+      </c>
+      <c r="H14" s="6">
+        <v>87</v>
+      </c>
+      <c r="I14" s="6">
+        <v>45</v>
+      </c>
+      <c r="J14" s="6">
+        <v>50</v>
+      </c>
+      <c r="K14" s="7">
+        <f t="shared" si="4"/>
+        <v>258</v>
+      </c>
+      <c r="L14" s="6">
+        <f t="shared" si="0"/>
+        <v>270.89999999999998</v>
+      </c>
+      <c r="M14" s="6">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="N14" s="6">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+      <c r="O14" s="6">
+        <f t="shared" si="3"/>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="F16" s="5" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="17" spans="6:12" x14ac:dyDescent="0.25">
+      <c r="F17" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="G17" s="9">
+        <f>AVERAGE(G8:G14)</f>
+        <v>66.428571428571431</v>
+      </c>
+      <c r="H17" s="9">
+        <f>AVERAGE(H8:H14)</f>
+        <v>84.571428571428569</v>
+      </c>
+      <c r="I17" s="9">
+        <f>AVERAGE(I8:I14)</f>
+        <v>67.571428571428569</v>
+      </c>
+      <c r="J17" s="9">
+        <f>AVERAGE(J8:J14)</f>
+        <v>39.285714285714285</v>
+      </c>
+      <c r="K17" s="9">
+        <f>AVERAGE(K8:K14)</f>
+        <v>257.85714285714283</v>
+      </c>
+      <c r="L17" s="9">
+        <f t="shared" si="0"/>
+        <v>270.75</v>
+      </c>
+    </row>
+    <row r="18" spans="6:12" x14ac:dyDescent="0.25">
+      <c r="F18" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="G18" s="6">
+        <f t="shared" ref="G18:L18" si="5">MIN(G8:G14)</f>
+        <v>40</v>
+      </c>
+      <c r="H18" s="6">
+        <f t="shared" si="5"/>
+        <v>67</v>
+      </c>
+      <c r="I18" s="6">
+        <f t="shared" si="5"/>
+        <v>44</v>
+      </c>
+      <c r="J18" s="6">
+        <f t="shared" si="5"/>
+        <v>0</v>
+      </c>
+      <c r="K18" s="6">
+        <f t="shared" si="5"/>
+        <v>185</v>
+      </c>
+      <c r="L18" s="6">
+        <f t="shared" si="5"/>
+        <v>194.25</v>
+      </c>
+    </row>
+    <row r="19" spans="6:12" x14ac:dyDescent="0.25">
+      <c r="F19" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="G19" s="6">
+        <f t="shared" ref="G19:L19" si="6">MAX(G8:G14)</f>
+        <v>77</v>
+      </c>
+      <c r="H19" s="6">
+        <f t="shared" si="6"/>
+        <v>98</v>
+      </c>
+      <c r="I19" s="6">
+        <f t="shared" si="6"/>
+        <v>98</v>
+      </c>
+      <c r="J19" s="6">
+        <f t="shared" si="6"/>
+        <v>159</v>
+      </c>
+      <c r="K19" s="6">
+        <f t="shared" si="6"/>
+        <v>357</v>
+      </c>
+      <c r="L19" s="6">
+        <f t="shared" si="6"/>
+        <v>374.85</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
task completed using countif and rank.eq formulas
</commit_message>
<xml_diff>
--- a/da20_excel_task1.xlsx
+++ b/da20_excel_task1.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\DA20\Git_hub\da20_excel_task1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01BEACA7-226F-4906-882A-FF0B48592D8E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F539163-AC2E-465F-BF6C-E910287031F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="10245" yWindow="0" windowWidth="10245" windowHeight="10920" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Task1" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="23">
   <si>
     <t>tax</t>
   </si>
@@ -83,9 +83,6 @@
     <t>sony</t>
   </si>
   <si>
-    <t>task</t>
-  </si>
-  <si>
     <t>haier1</t>
   </si>
   <si>
@@ -107,24 +104,17 @@
     <t>max</t>
   </si>
   <si>
-    <t>da20_excel_task1</t>
+    <t>Task</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -163,7 +153,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4"/>
+        <fgColor theme="7" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -242,13 +232,13 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -531,10 +521,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="C4:P19"/>
+  <dimension ref="F4:P19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N17" sqref="N17"/>
+    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -544,11 +534,13 @@
     <col min="7" max="8" width="9.140625" style="1"/>
     <col min="9" max="9" width="11.140625" style="1" customWidth="1"/>
     <col min="10" max="11" width="9.140625" style="1"/>
-    <col min="12" max="12" width="13.28515625" style="1" customWidth="1"/>
-    <col min="13" max="16384" width="9.140625" style="1"/>
+    <col min="12" max="12" width="15.5703125" style="1" customWidth="1"/>
+    <col min="13" max="18" width="9.140625" style="1"/>
+    <col min="19" max="19" width="34.5703125" style="1" customWidth="1"/>
+    <col min="20" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="4" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="4" spans="6:16" x14ac:dyDescent="0.25">
       <c r="J4" s="2" t="s">
         <v>0</v>
       </c>
@@ -556,12 +548,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="5" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="C5" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="7" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="7" spans="6:16" x14ac:dyDescent="0.25">
       <c r="F7" s="4" t="s">
         <v>1</v>
       </c>
@@ -592,8 +579,11 @@
       <c r="O7" s="4" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="8" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="P7" s="10" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="6:16" x14ac:dyDescent="0.25">
       <c r="F8" s="5" t="s">
         <v>11</v>
       </c>
@@ -629,8 +619,12 @@
         <f>RANK(M8,M$8:M$14,1)</f>
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="P8" s="6">
+        <f xml:space="preserve"> N8+COUNTIF($L$8:L8,L8)-1</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="6:16" x14ac:dyDescent="0.25">
       <c r="F9" s="5" t="s">
         <v>12</v>
       </c>
@@ -666,8 +660,12 @@
         <f t="shared" ref="O9:O14" si="3">RANK(M9,M$8:M$14,1)</f>
         <v>6</v>
       </c>
-    </row>
-    <row r="10" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="P9" s="6">
+        <f xml:space="preserve"> N9+COUNTIF($L$8:L9,L9)-1</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="6:16" x14ac:dyDescent="0.25">
       <c r="F10" s="5" t="s">
         <v>13</v>
       </c>
@@ -703,8 +701,12 @@
         <f t="shared" si="3"/>
         <v>7</v>
       </c>
-    </row>
-    <row r="11" spans="3:16" x14ac:dyDescent="0.25">
+      <c r="P10" s="6">
+        <f xml:space="preserve"> N10+COUNTIF($L$8:L10,L10)-1</f>
+        <v>7</v>
+      </c>
+    </row>
+    <row r="11" spans="6:16" x14ac:dyDescent="0.25">
       <c r="F11" s="5" t="s">
         <v>14</v>
       </c>
@@ -740,13 +742,14 @@
         <f t="shared" si="3"/>
         <v>2</v>
       </c>
-      <c r="P11" s="1" t="s">
+      <c r="P11" s="6">
+        <f xml:space="preserve"> N11+COUNTIF($L$8:L11,L11)-1</f>
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="6:16" x14ac:dyDescent="0.25">
+      <c r="F12" s="5" t="s">
         <v>15</v>
-      </c>
-    </row>
-    <row r="12" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="F12" s="5" t="s">
-        <v>16</v>
       </c>
       <c r="G12" s="6">
         <v>76</v>
@@ -780,13 +783,14 @@
         <f t="shared" si="3"/>
         <v>4</v>
       </c>
-      <c r="P12" s="1">
+      <c r="P12" s="6">
+        <f xml:space="preserve"> N12+COUNTIF($L$8:L12,L12)-1</f>
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="13" spans="6:16" x14ac:dyDescent="0.25">
       <c r="F13" s="5" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G13" s="6">
         <v>76</v>
@@ -820,13 +824,14 @@
         <f t="shared" si="3"/>
         <v>4</v>
       </c>
-      <c r="P13" s="1">
+      <c r="P13" s="6">
+        <f xml:space="preserve"> N13+COUNTIF($L$8:L13,L13)-1</f>
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="14" spans="6:16" x14ac:dyDescent="0.25">
       <c r="F14" s="5" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="G14" s="6">
         <v>76</v>
@@ -860,44 +865,48 @@
         <f t="shared" si="3"/>
         <v>3</v>
       </c>
-    </row>
-    <row r="16" spans="3:16" x14ac:dyDescent="0.25">
-      <c r="F16" s="5" t="s">
+      <c r="P14" s="6">
+        <f xml:space="preserve"> N14+COUNTIF($L$8:L14,L14)-1</f>
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="6:16" x14ac:dyDescent="0.25">
+      <c r="F16" s="4" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="6:12" x14ac:dyDescent="0.25">
+      <c r="F17" s="5" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="17" spans="6:12" x14ac:dyDescent="0.25">
-      <c r="F17" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="G17" s="9">
+      <c r="G17" s="8">
         <f>AVERAGE(G8:G14)</f>
         <v>66.428571428571431</v>
       </c>
-      <c r="H17" s="9">
+      <c r="H17" s="8">
         <f>AVERAGE(H8:H14)</f>
         <v>84.571428571428569</v>
       </c>
-      <c r="I17" s="9">
+      <c r="I17" s="8">
         <f>AVERAGE(I8:I14)</f>
         <v>67.571428571428569</v>
       </c>
-      <c r="J17" s="9">
+      <c r="J17" s="8">
         <f>AVERAGE(J8:J14)</f>
         <v>39.285714285714285</v>
       </c>
-      <c r="K17" s="9">
+      <c r="K17" s="8">
         <f>AVERAGE(K8:K14)</f>
         <v>257.85714285714283</v>
       </c>
-      <c r="L17" s="9">
+      <c r="L17" s="8">
         <f t="shared" si="0"/>
         <v>270.75</v>
       </c>
     </row>
     <row r="18" spans="6:12" x14ac:dyDescent="0.25">
       <c r="F18" s="5" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="G18" s="6">
         <f t="shared" ref="G18:L18" si="5">MIN(G8:G14)</f>
@@ -925,8 +934,8 @@
       </c>
     </row>
     <row r="19" spans="6:12" x14ac:dyDescent="0.25">
-      <c r="F19" s="10" t="s">
-        <v>22</v>
+      <c r="F19" s="9" t="s">
+        <v>21</v>
       </c>
       <c r="G19" s="6">
         <f t="shared" ref="G19:L19" si="6">MAX(G8:G14)</f>

</xml_diff>